<commit_message>
Added in month as a factor
</commit_message>
<xml_diff>
--- a/Data/PNMS Pelagic Fish Reproduction_Samples_First batch_March 2022.xlsx
+++ b/Data/PNMS Pelagic Fish Reproduction_Samples_First batch_March 2022.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Palau\Research\PNMS Research\PICRC led PNMS Research\Tuna Reproduction\Gonad research\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Palau\Research\PNMS Research\PICRC led PNMS Research\Tuna Reproduction\Gonad research\Data\PNMS_Tuna_Gonad\PNMS_Tuna_Gonad\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7052F6FA-085E-44EA-89C4-0B69290D6F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C36C8D-B89B-4105-BF41-1B0224C2B347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{51ECF0B3-72A2-4D3B-A0AA-D0F06562B8F4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Bio_samples" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Bio_samples!$A$1:$I$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Bio_samples!$A$1:$K$73</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="109">
   <si>
     <t>Date</t>
   </si>
@@ -391,6 +391,12 @@
       </rPr>
       <t>No 2_2_BE found in batch</t>
     </r>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
   </si>
 </sst>
 </file>
@@ -483,14 +489,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -809,10 +815,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:K78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+      <selection activeCell="A2" sqref="A2:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -823,12 +829,12 @@
     <col min="4" max="4" width="6.6640625" customWidth="1"/>
     <col min="5" max="5" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.109375" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="60.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22" customWidth="1"/>
+    <col min="7" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="60.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -851,11 +857,17 @@
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="8"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -877,12 +889,14 @@
       <c r="G2" s="5">
         <v>508</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K2" s="7"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -904,10 +918,12 @@
       <c r="G3" s="3">
         <v>290</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -929,10 +945,12 @@
       <c r="G4" s="3">
         <v>112.3</v>
       </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -954,10 +972,12 @@
       <c r="G5" s="3">
         <v>319.89999999999998</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -979,10 +999,12 @@
       <c r="G6" s="3">
         <v>285.60000000000002</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -1004,10 +1026,12 @@
       <c r="G7" s="3">
         <v>285.7</v>
       </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1029,10 +1053,12 @@
       <c r="G8" s="3">
         <v>251.4</v>
       </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
@@ -1055,8 +1081,10 @@
         <v>269.39999999999998</v>
       </c>
       <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
@@ -1079,8 +1107,10 @@
         <v>214.1</v>
       </c>
       <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -1103,8 +1133,10 @@
         <v>296.8</v>
       </c>
       <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
@@ -1127,8 +1159,10 @@
         <v>347.2</v>
       </c>
       <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>20</v>
       </c>
@@ -1151,8 +1185,10 @@
         <v>472.7</v>
       </c>
       <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
@@ -1175,8 +1211,10 @@
         <v>257.5</v>
       </c>
       <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
@@ -1199,8 +1237,10 @@
         <v>277.39999999999998</v>
       </c>
       <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
@@ -1223,8 +1263,10 @@
         <v>211.7</v>
       </c>
       <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
@@ -1247,8 +1289,10 @@
         <v>94</v>
       </c>
       <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>28</v>
       </c>
@@ -1271,34 +1315,38 @@
         <v>311.60000000000002</v>
       </c>
       <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="9">
         <v>122</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="9">
         <v>31.8</v>
       </c>
-      <c r="F19" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="11">
+      <c r="F19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="9">
         <v>292.39999999999998</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>28</v>
       </c>
@@ -1321,8 +1369,10 @@
         <v>276.89999999999998</v>
       </c>
       <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
@@ -1345,8 +1395,10 @@
         <v>250.6</v>
       </c>
       <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>35</v>
       </c>
@@ -1369,8 +1421,10 @@
         <v>97.1</v>
       </c>
       <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>35</v>
       </c>
@@ -1393,8 +1447,10 @@
         <v>185.1</v>
       </c>
       <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>35</v>
       </c>
@@ -1417,8 +1473,10 @@
         <v>237.8</v>
       </c>
       <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
@@ -1441,8 +1499,10 @@
         <v>208.4</v>
       </c>
       <c r="H25" s="3"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>35</v>
       </c>
@@ -1465,8 +1525,10 @@
         <v>187.5</v>
       </c>
       <c r="H26" s="3"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>35</v>
       </c>
@@ -1489,8 +1551,10 @@
         <v>221.4</v>
       </c>
       <c r="H27" s="3"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>35</v>
       </c>
@@ -1513,8 +1577,10 @@
         <v>199.2</v>
       </c>
       <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
@@ -1537,8 +1603,10 @@
         <v>448.8</v>
       </c>
       <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>35</v>
       </c>
@@ -1561,8 +1629,10 @@
         <v>109</v>
       </c>
       <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>45</v>
       </c>
@@ -1584,9 +1654,11 @@
       <c r="G31" s="6">
         <v>84.5</v>
       </c>
-      <c r="H31" s="3"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>45</v>
       </c>
@@ -1608,9 +1680,11 @@
       <c r="G32" s="6">
         <v>253.6</v>
       </c>
-      <c r="H32" s="3"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>45</v>
       </c>
@@ -1632,9 +1706,11 @@
       <c r="G33" s="6">
         <v>751</v>
       </c>
-      <c r="H33" s="3"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>45</v>
       </c>
@@ -1656,9 +1732,11 @@
       <c r="G34" s="6">
         <v>280.5</v>
       </c>
-      <c r="H34" s="3"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>45</v>
       </c>
@@ -1680,9 +1758,11 @@
       <c r="G35" s="6">
         <v>430.2</v>
       </c>
-      <c r="H35" s="3"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>45</v>
       </c>
@@ -1704,9 +1784,11 @@
       <c r="G36" s="6">
         <v>271.10000000000002</v>
       </c>
-      <c r="H36" s="3"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>45</v>
       </c>
@@ -1728,9 +1810,11 @@
       <c r="G37" s="6">
         <v>403.7</v>
       </c>
-      <c r="H37" s="3"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>45</v>
       </c>
@@ -1752,9 +1836,11 @@
       <c r="G38" s="6">
         <v>330.2</v>
       </c>
-      <c r="H38" s="3"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>54</v>
       </c>
@@ -1776,9 +1862,11 @@
       <c r="G39" s="6">
         <v>111.5</v>
       </c>
-      <c r="H39" s="3"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>54</v>
       </c>
@@ -1800,9 +1888,11 @@
       <c r="G40" s="6">
         <v>179</v>
       </c>
-      <c r="H40" s="3"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="3"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>54</v>
       </c>
@@ -1824,9 +1914,11 @@
       <c r="G41" s="6">
         <v>179.7</v>
       </c>
-      <c r="H41" s="3"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="3"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>54</v>
       </c>
@@ -1848,9 +1940,11 @@
       <c r="G42" s="6">
         <v>362.7</v>
       </c>
-      <c r="H42" s="3"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="3"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>54</v>
       </c>
@@ -1872,9 +1966,11 @@
       <c r="G43" s="6">
         <v>139.5</v>
       </c>
-      <c r="H43" s="3"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="3"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>54</v>
       </c>
@@ -1896,9 +1992,11 @@
       <c r="G44" s="6">
         <v>170.5</v>
       </c>
-      <c r="H44" s="3"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="3"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>54</v>
       </c>
@@ -1920,9 +2018,11 @@
       <c r="G45" s="6">
         <v>296.3</v>
       </c>
-      <c r="H45" s="3"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="3"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>60</v>
       </c>
@@ -1944,9 +2044,11 @@
       <c r="G46" s="6">
         <v>97.3</v>
       </c>
-      <c r="H46" s="3"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="3"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>60</v>
       </c>
@@ -1968,9 +2070,11 @@
       <c r="G47" s="6">
         <v>224.6</v>
       </c>
-      <c r="H47" s="3"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="3"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>60</v>
       </c>
@@ -1992,9 +2096,11 @@
       <c r="G48" s="6">
         <v>245.8</v>
       </c>
-      <c r="H48" s="3"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="3"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>60</v>
       </c>
@@ -2016,9 +2122,11 @@
       <c r="G49" s="6">
         <v>196.6</v>
       </c>
-      <c r="H49" s="3"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="3"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>60</v>
       </c>
@@ -2040,9 +2148,11 @@
       <c r="G50" s="6">
         <v>323.2</v>
       </c>
-      <c r="H50" s="3"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="3"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
         <v>68</v>
       </c>
@@ -2064,9 +2174,11 @@
       <c r="G51" s="6">
         <v>168.4</v>
       </c>
-      <c r="H51" s="3"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="3"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>68</v>
       </c>
@@ -2088,9 +2200,11 @@
       <c r="G52" s="6">
         <v>190.2</v>
       </c>
-      <c r="H52" s="3"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="3"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>68</v>
       </c>
@@ -2112,9 +2226,11 @@
       <c r="G53" s="6">
         <v>251</v>
       </c>
-      <c r="H53" s="3"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="3"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>68</v>
       </c>
@@ -2137,8 +2253,10 @@
         <v>341.1</v>
       </c>
       <c r="H54" s="3"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>68</v>
       </c>
@@ -2161,8 +2279,10 @@
         <v>197.2</v>
       </c>
       <c r="H55" s="3"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>68</v>
       </c>
@@ -2185,8 +2305,10 @@
         <v>180.3</v>
       </c>
       <c r="H56" s="3"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>75</v>
       </c>
@@ -2208,9 +2330,11 @@
       <c r="G57" s="6">
         <v>350.6</v>
       </c>
-      <c r="H57" s="3"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+      <c r="J57" s="3"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>75</v>
       </c>
@@ -2232,9 +2356,11 @@
       <c r="G58" s="6">
         <v>253.3</v>
       </c>
-      <c r="H58" s="3"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="3"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
         <v>75</v>
       </c>
@@ -2256,9 +2382,11 @@
       <c r="G59" s="6">
         <v>255</v>
       </c>
-      <c r="H59" s="3"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="3"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>75</v>
       </c>
@@ -2280,9 +2408,11 @@
       <c r="G60" s="6">
         <v>585.20000000000005</v>
       </c>
-      <c r="H60" s="3"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="3"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>75</v>
       </c>
@@ -2304,9 +2434,11 @@
       <c r="G61" s="6">
         <v>297.8</v>
       </c>
-      <c r="H61" s="3"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H61" s="6"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="3"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>75</v>
       </c>
@@ -2329,8 +2461,10 @@
         <v>82</v>
       </c>
       <c r="H62" s="3"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>83</v>
       </c>
@@ -2352,9 +2486,11 @@
       <c r="G63" s="6">
         <v>267.2</v>
       </c>
-      <c r="H63" s="3"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="3"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>83</v>
       </c>
@@ -2376,9 +2512,11 @@
       <c r="G64" s="6">
         <v>255.5</v>
       </c>
-      <c r="H64" s="3"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="3"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
         <v>83</v>
       </c>
@@ -2400,9 +2538,11 @@
       <c r="G65" s="6">
         <v>277.60000000000002</v>
       </c>
-      <c r="H65" s="3"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="3"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
         <v>83</v>
       </c>
@@ -2424,9 +2564,11 @@
       <c r="G66" s="6">
         <v>179.2</v>
       </c>
-      <c r="H66" s="3"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="3"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
         <v>83</v>
       </c>
@@ -2448,9 +2590,11 @@
       <c r="G67" s="6">
         <v>154.1</v>
       </c>
-      <c r="H67" s="3"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="3"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
         <v>83</v>
       </c>
@@ -2472,61 +2616,67 @@
       <c r="G68" s="6">
         <v>190.1</v>
       </c>
-      <c r="H68" s="3"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A69" s="12" t="s">
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="3"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B69" s="12" t="s">
+      <c r="B69" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C69" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D69" s="12">
+      <c r="C69" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="10">
         <v>107</v>
       </c>
-      <c r="E69" s="12">
+      <c r="E69" s="10">
         <v>26.3</v>
       </c>
-      <c r="F69" s="12" t="s">
+      <c r="F69" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G69" s="12">
+      <c r="G69" s="10">
         <v>171.9</v>
       </c>
-      <c r="H69" s="3" t="s">
+      <c r="H69" s="10"/>
+      <c r="I69" s="10"/>
+      <c r="J69" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A70" s="12" t="s">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B70" s="12" t="s">
+      <c r="B70" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="C70" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D70" s="12">
+      <c r="C70" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="10">
         <v>105</v>
       </c>
-      <c r="E70" s="12">
+      <c r="E70" s="10">
         <v>23.5</v>
       </c>
-      <c r="F70" s="12" t="s">
+      <c r="F70" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G70" s="12">
+      <c r="G70" s="10">
         <v>150.1</v>
       </c>
-      <c r="H70" s="3" t="s">
+      <c r="H70" s="10"/>
+      <c r="I70" s="10"/>
+      <c r="J70" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>90</v>
       </c>
@@ -2548,11 +2698,13 @@
       <c r="G71" s="6">
         <v>71.400000000000006</v>
       </c>
-      <c r="H71" s="3" t="s">
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
         <v>90</v>
       </c>
@@ -2574,11 +2726,13 @@
       <c r="G72" s="6">
         <v>343.6</v>
       </c>
-      <c r="H72" s="3" t="s">
+      <c r="H72" s="6"/>
+      <c r="I72" s="6"/>
+      <c r="J72" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
         <v>90</v>
       </c>
@@ -2600,11 +2754,13 @@
       <c r="G73" s="6">
         <v>74.3</v>
       </c>
-      <c r="H73" s="3" t="s">
+      <c r="H73" s="6"/>
+      <c r="I73" s="6"/>
+      <c r="J73" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
         <v>96</v>
       </c>
@@ -2626,9 +2782,11 @@
       <c r="G74" s="6">
         <v>140.19999999999999</v>
       </c>
-      <c r="H74" s="3"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="3"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
         <v>96</v>
       </c>
@@ -2650,9 +2808,11 @@
       <c r="G75" s="6">
         <v>696.3</v>
       </c>
-      <c r="H75" s="3"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="3"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
         <v>96</v>
       </c>
@@ -2674,9 +2834,11 @@
       <c r="G76" s="6">
         <v>360.2</v>
       </c>
-      <c r="H76" s="3"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="3"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="6" t="s">
         <v>96</v>
       </c>
@@ -2698,9 +2860,11 @@
       <c r="G77" s="6">
         <v>217.6</v>
       </c>
-      <c r="H77" s="3"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="3"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
         <v>96</v>
       </c>
@@ -2722,12 +2886,14 @@
       <c r="G78" s="6">
         <v>647</v>
       </c>
-      <c r="H78" s="3"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I73" xr:uid="{7E9E4142-BBB9-4D98-AC15-E639C15E6487}"/>
+  <autoFilter ref="A1:K73" xr:uid="{7E9E4142-BBB9-4D98-AC15-E639C15E6487}"/>
   <mergeCells count="1">
-    <mergeCell ref="H2:H8"/>
+    <mergeCell ref="J2:J8"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.5" right="0.4375" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>